<commit_message>
A bit of cleaning and analytics
</commit_message>
<xml_diff>
--- a/data/apmo_reports.xlsx
+++ b/data/apmo_reports.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,21 +20,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t xml:space="preserve">General information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">By country alphabetical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">By country rank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">By problem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">By medals</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="7">
+  <si>
+    <t xml:space="preserve">Score Table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country Rankings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TXT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSON</t>
   </si>
 </sst>
 </file>
@@ -49,6 +55,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -108,9 +115,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -130,18 +141,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.4642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -154,166 +164,311 @@
       <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1989</v>
       </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1990</v>
       </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1991</v>
       </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>1992</v>
       </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>1993</v>
       </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>1994</v>
       </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>1995</v>
       </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>1996</v>
       </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>1997</v>
       </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>1998</v>
       </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>1999</v>
       </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>2000</v>
       </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>2001</v>
       </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>2002</v>
       </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>2003</v>
       </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>2004</v>
       </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>2005</v>
       </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>2006</v>
       </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>2007</v>
       </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>2008</v>
       </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>2009</v>
       </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>2010</v>
       </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>2011</v>
       </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>2012</v>
       </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>2013</v>
       </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>2014</v>
       </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>2015</v>
       </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>2016</v>
       </c>
+      <c r="B29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>2017</v>
       </c>
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>2018</v>
       </c>
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>2019</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>